<commit_message>
Better data processing, sankey updates
</commit_message>
<xml_diff>
--- a/public/data/college-majors/95-96/by-98-major12.xlsx
+++ b/public/data/college-majors/95-96/by-98-major12.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chase\Dropbox\School\Visualization\data\college-majors\2001\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chase\Dropbox\School\Visualization\visualization-oss\public\data\college-majors\95-96\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22545" windowHeight="9180"/>
   </bookViews>
   <sheets>
     <sheet name="Output (3)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1535,9 +1535,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>